<commit_message>
add few things by RYAN
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabin\Desktop\2810ICT_PartB-Statistical-Data-Analysis-and-Presentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryankim/Documents/2810ICT_PartB-Statistical-Data-Analysis-and-Presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4872BD1-060C-4578-940B-900EE3A16634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBD902A-B423-5D41-9D39-A9255CFC2420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -280,17 +280,20 @@
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="7"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -604,12 +607,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -630,18 +645,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1045,24 +1048,24 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.4140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
-    <col min="42" max="42" width="2.75" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="2.6640625" style="1"/>
+    <col min="42" max="42" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.25">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
         <v>42</v>
       </c>
@@ -1072,14 +1075,14 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="33" t="s">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1087,37 +1090,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="30" t="s">
+      <c r="V2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
+      <c r="AA2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
         <v>4</v>
@@ -1130,23 +1133,23 @@
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="36" t="s">
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="29" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1172,13 +1175,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="35"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1379,8 +1382,9 @@
       <c r="G5" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1399,8 +1403,9 @@
       <c r="G6" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -1419,8 +1424,9 @@
       <c r="G7" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -1439,8 +1445,9 @@
       <c r="G8" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1459,8 +1466,9 @@
       <c r="G9" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1479,8 +1487,9 @@
       <c r="G10" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -1499,8 +1508,9 @@
       <c r="G11" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -1519,8 +1529,9 @@
       <c r="G12" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -1539,8 +1550,9 @@
       <c r="G13" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -1559,8 +1571,9 @@
       <c r="G14" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -1579,8 +1592,9 @@
       <c r="G15" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -1619,8 +1633,9 @@
       <c r="G17" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
@@ -1639,8 +1654,9 @@
       <c r="G18" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M18" s="17"/>
+    </row>
+    <row r="19" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
@@ -1659,8 +1675,9 @@
       <c r="G19" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="L19" s="17"/>
+    </row>
+    <row r="20" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>29</v>
       </c>
@@ -1679,8 +1696,9 @@
       <c r="G20" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="N20" s="17"/>
+    </row>
+    <row r="21" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>30</v>
       </c>
@@ -1699,8 +1717,9 @@
       <c r="G21" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="N21" s="17"/>
+    </row>
+    <row r="22" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>31</v>
       </c>
@@ -1719,8 +1738,9 @@
       <c r="G22" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P22" s="17"/>
+    </row>
+    <row r="23" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>32</v>
       </c>
@@ -1739,8 +1759,9 @@
       <c r="G23" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>33</v>
       </c>
@@ -1759,8 +1780,9 @@
       <c r="G24" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>34</v>
       </c>
@@ -1779,8 +1801,9 @@
       <c r="G25" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>35</v>
       </c>
@@ -1799,8 +1822,9 @@
       <c r="G26" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>36</v>
       </c>
@@ -1819,8 +1843,9 @@
       <c r="G27" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>37</v>
       </c>
@@ -1839,8 +1864,9 @@
       <c r="G28" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>38</v>
       </c>
@@ -1859,8 +1885,9 @@
       <c r="G29" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q29" s="17"/>
+    </row>
+    <row r="30" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>39</v>
       </c>
@@ -1879,8 +1906,9 @@
       <c r="G30" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q30" s="17"/>
+    </row>
+    <row r="31" spans="2:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
@@ -1899,8 +1927,9 @@
       <c r="G31" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q31" s="17"/>
+    </row>
+    <row r="32" spans="2:17" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>41</v>
       </c>
@@ -1920,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1928,7 +1957,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1936,7 +1965,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1944,7 +1973,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1952,7 +1981,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1960,7 +1989,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1968,7 +1997,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1978,24 +2007,24 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO39">
+  <conditionalFormatting sqref="H16:BO16 H5:H15 J5:BO15 H32:BO39 H17:L18 N17:BO18 H19:K19 M19:BO19 H20:M21 O20:BO21 H22:O22 Q22:BO22 I23:BO28 H29:P31 R29:BO31">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2027,7 +2056,7 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 I5:I15 M17:M18 L19 N20:N21 P22 H23:H28 Q29:Q31" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>

</xml_diff>